<commit_message>
Update to Pws version
</commit_message>
<xml_diff>
--- a/Fdata.xlsx
+++ b/Fdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB5D5A-6AE5-403A-BC14-1286BA868D17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676DA036-6C4A-46C9-B15D-D906E13916E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Vgs</t>
   </si>
@@ -66,9 +66,6 @@
     <t>3 - Rand (3.875)</t>
   </si>
   <si>
-    <t>4 - Rand Vgs</t>
-  </si>
-  <si>
     <t>5 - Varying Vds (4.670, ~23)</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>&lt;- e</t>
   </si>
   <si>
-    <t>&lt;- a                   Graphs to Show -&gt;</t>
-  </si>
-  <si>
     <t>Plot Vgs</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
     <t>&lt;- chart vds max</t>
   </si>
   <si>
-    <t>Thrash</t>
-  </si>
-  <si>
     <t>&lt;- marker size</t>
   </si>
   <si>
@@ -133,6 +124,73 @@
   </si>
   <si>
     <t>Options</t>
+  </si>
+  <si>
+    <t>Stash</t>
+  </si>
+  <si>
+    <t>Stash Notes</t>
+  </si>
+  <si>
+    <t>This is a place to stash run options</t>
+  </si>
+  <si>
+    <t>&lt;- Exponent on Vtj, const b. Kwadratic Vgs</t>
+  </si>
+  <si>
+    <t>Copy Runs to &lt;- a and onward</t>
+  </si>
+  <si>
+    <t>&lt;- T^2.3 with quadratic Vgs, e can be &lt;0</t>
+  </si>
+  <si>
+    <t>&lt;- Exponent on Vtj, const b. Linear Vgs. e can be &lt;0</t>
+  </si>
+  <si>
+    <t>Regression Options</t>
+  </si>
+  <si>
+    <t>Style Options</t>
+  </si>
+  <si>
+    <t>Image Options</t>
+  </si>
+  <si>
+    <t>&lt;- Image Elevation</t>
+  </si>
+  <si>
+    <t>&lt;- Image Azimuth</t>
+  </si>
+  <si>
+    <t>&lt;- Image Title (0 for no image save)</t>
+  </si>
+  <si>
+    <t>&lt;- T^2.3 with linear Vgs, e can be &lt;0</t>
+  </si>
+  <si>
+    <t>&lt;- Model 1</t>
+  </si>
+  <si>
+    <t>&lt;- Model 2</t>
+  </si>
+  <si>
+    <t>&lt;- Model 3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;- a                  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Graphs to Show -&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -144,8 +202,16 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -173,12 +239,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -186,9 +253,6 @@
   <dxfs count="10">
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -214,6 +278,9 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -228,22 +295,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3DC3BBE-32BD-4EFF-AF7D-892BD187032E}" name="Tabel1" displayName="Tabel1" ref="A1:M151" totalsRowShown="0">
-  <autoFilter ref="A1:M151" xr:uid="{AB1DCA6B-C573-4F9A-9074-2DA1A149F8DD}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{5A17D80A-F3EF-4BF7-AABE-25DFD97858F6}" name="Vgs" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{FAADD048-94F2-404C-A9E0-FA5F4EAD378D}" name="Vds" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{1BCB5B24-AC82-408A-8F20-15349CE11713}" name="Ids" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{5F3B280B-3A0A-4839-8835-16FDD782B7C3}" name="Ta" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{2B23BA03-D4EE-48AB-8FE7-060B66A5A6F2}" name="Tc" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{513803C8-AF9A-4638-87F0-CA9CEB55AF4E}" name="Trise" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{F84A1DC0-E431-4741-AEFF-18BA5A8F9E34}" name="Tfall" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{10317700-BD6D-4814-B1E5-21AA06CB821A}" name="Fmax" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3DC3BBE-32BD-4EFF-AF7D-892BD187032E}" name="Tabel1" displayName="Tabel1" ref="A1:N144" totalsRowShown="0">
+  <autoFilter ref="A1:N144" xr:uid="{AB1DCA6B-C573-4F9A-9074-2DA1A149F8DD}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{5A17D80A-F3EF-4BF7-AABE-25DFD97858F6}" name="Vgs" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FAADD048-94F2-404C-A9E0-FA5F4EAD378D}" name="Vds" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{1BCB5B24-AC82-408A-8F20-15349CE11713}" name="Ids" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5F3B280B-3A0A-4839-8835-16FDD782B7C3}" name="Ta" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{2B23BA03-D4EE-48AB-8FE7-060B66A5A6F2}" name="Tc" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{513803C8-AF9A-4638-87F0-CA9CEB55AF4E}" name="Trise" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F84A1DC0-E431-4741-AEFF-18BA5A8F9E34}" name="Tfall" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{10317700-BD6D-4814-B1E5-21AA06CB821A}" name="Fmax" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{2C105548-C8A8-42DC-9EE6-38EBED037B4A}" name="Measurment Sets"/>
     <tableColumn id="10" xr3:uid="{2C6D2759-86A9-4C1E-B946-67E8C634FA83}" name="Options" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{FFD94DC3-A323-4273-9C59-82588A5BF7CC}" name="Note"/>
     <tableColumn id="12" xr3:uid="{C1304E0F-94A0-48CA-85AC-9551D33316B1}" name="Plot Vgs" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{D3C6E1D3-D70D-4ABD-B685-C0A2CC9A9E96}" name="Thrash"/>
+    <tableColumn id="18" xr3:uid="{D3C6E1D3-D70D-4ABD-B685-C0A2CC9A9E96}" name="Stash"/>
+    <tableColumn id="13" xr3:uid="{784AB07E-F9E7-4AD6-883B-10FEEAB2D9F7}" name="Stash Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -512,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:N144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,9 +594,12 @@
     <col min="10" max="10" width="21.5703125" style="4" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="47.140625" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,22 +625,25 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4.99</v>
       </c>
@@ -598,16 +672,19 @@
         <v>9</v>
       </c>
       <c r="J2" s="4">
-        <v>6.9643331999999996</v>
+        <v>5.500000002048</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4.99</v>
       </c>
@@ -633,16 +710,19 @@
         <v>3.7730000000000001</v>
       </c>
       <c r="J3" s="4">
-        <v>2.83033331999999</v>
+        <v>3.1936320004095999</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="1">
         <v>4.67</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4.99</v>
       </c>
@@ -668,16 +748,16 @@
         <v>3.6909999999999998</v>
       </c>
       <c r="J4" s="4">
-        <v>0.50408971999999996</v>
+        <v>0.10298397196287901</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" s="1">
         <v>3.875</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4.99</v>
       </c>
@@ -703,13 +783,19 @@
         <v>3.6150000000000002</v>
       </c>
       <c r="J5" s="4">
-        <v>38.333333199999998</v>
+        <v>22.679999995904002</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4">
+        <v>6.8635058000000004</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4.99</v>
       </c>
@@ -735,13 +821,16 @@
         <v>3.5950000000000002</v>
       </c>
       <c r="J6" s="4">
-        <v>-4.8666666000000003</v>
+        <v>-0.34999999897599898</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2.8318966799999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4.99</v>
       </c>
@@ -770,10 +859,13 @@
         <v>300</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0.49443307999999903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4.99</v>
       </c>
@@ -799,13 +891,16 @@
         <v>2.9809999999999999</v>
       </c>
       <c r="J8" s="4">
-        <v>2.2999999999999998</v>
+        <v>-0.53681599897599996</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="M8" s="4">
+        <v>38.033333199999902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4.99</v>
       </c>
@@ -831,13 +926,16 @@
         <v>2.839</v>
       </c>
       <c r="J9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="M9" s="4">
+        <v>-4.8666666000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4.99</v>
       </c>
@@ -862,8 +960,14 @@
       <c r="H10" s="1">
         <v>2.7389999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4.99</v>
       </c>
@@ -889,13 +993,16 @@
         <v>2.5830000000000002</v>
       </c>
       <c r="J11" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4.99</v>
       </c>
@@ -924,10 +1031,13 @@
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="M12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4.99</v>
       </c>
@@ -956,10 +1066,10 @@
         <v>0.3</v>
       </c>
       <c r="K13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4.99</v>
       </c>
@@ -988,10 +1098,16 @@
         <v>7</v>
       </c>
       <c r="K14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="M14" s="4">
+        <v>4.5653031999999998</v>
+      </c>
+      <c r="N14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4.99</v>
       </c>
@@ -1016,8 +1132,14 @@
       <c r="H15" s="1">
         <v>2.173</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" s="4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4.99</v>
       </c>
@@ -1046,10 +1168,13 @@
         <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="M16" s="4">
+        <v>-3.2647620000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4.99</v>
       </c>
@@ -1074,8 +1199,14 @@
       <c r="H17" s="1">
         <v>2.1419999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="4">
+        <v>35.666666800000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4.99</v>
       </c>
@@ -1100,8 +1231,17 @@
       <c r="H18" s="1">
         <v>2.1280000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>45</v>
+      </c>
+      <c r="M18" s="4">
+        <v>-4.8666666000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4.99</v>
       </c>
@@ -1126,8 +1266,17 @@
       <c r="H19" s="1">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="4">
+        <v>225</v>
+      </c>
+      <c r="K19" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4.99</v>
       </c>
@@ -1152,8 +1301,17 @@
       <c r="H20" s="1">
         <v>1.9990000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="4">
+        <v>-0.47620109999999899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4.99</v>
       </c>
@@ -1178,8 +1336,11 @@
       <c r="H21" s="1">
         <v>1.885</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4.99</v>
       </c>
@@ -1205,7 +1366,7 @@
         <v>1.8169999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4.99</v>
       </c>
@@ -1230,8 +1391,11 @@
       <c r="H23" s="1">
         <v>1.7609999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4.99</v>
       </c>
@@ -1257,7 +1421,7 @@
         <v>1.7110000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4.99</v>
       </c>
@@ -1283,7 +1447,7 @@
         <v>1.623</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4.99</v>
       </c>
@@ -1312,7 +1476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>4.99</v>
       </c>
@@ -1338,7 +1502,7 @@
         <v>2.0049999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4.99</v>
       </c>
@@ -1364,7 +1528,7 @@
         <v>2.069</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4.99</v>
       </c>
@@ -1390,7 +1554,7 @@
         <v>2.0409999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4.99</v>
       </c>
@@ -1416,7 +1580,7 @@
         <v>2.0779999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4.99</v>
       </c>
@@ -1442,7 +1606,7 @@
         <v>2.133</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>4.99</v>
       </c>
@@ -1467,8 +1631,14 @@
       <c r="H32" s="1">
         <v>2.0939999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M32" s="4">
+        <v>15.7753332</v>
+      </c>
+      <c r="N32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4.99</v>
       </c>
@@ -1493,8 +1663,11 @@
       <c r="H33" s="1">
         <v>2.1459999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M33" s="4">
+        <v>3.38050551999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4.99</v>
       </c>
@@ -1519,8 +1692,11 @@
       <c r="H34" s="1">
         <v>2.1840000000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M34" s="4">
+        <v>1.0258494600000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>4.99</v>
       </c>
@@ -1545,8 +1721,11 @@
       <c r="H35" s="1">
         <v>2.1890000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M35" s="4">
+        <v>37.333333199999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4.99</v>
       </c>
@@ -1571,8 +1750,11 @@
       <c r="H36" s="1">
         <v>2.1989999999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M36" s="4">
+        <v>-4.7666665999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>4.99</v>
       </c>
@@ -1597,8 +1779,11 @@
       <c r="H37" s="1">
         <v>2.2170000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M37" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>4.99</v>
       </c>
@@ -1626,8 +1811,11 @@
       <c r="I38" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M38" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>4.99</v>
       </c>
@@ -1652,8 +1840,11 @@
       <c r="H39" s="1">
         <v>2.641</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>4.99</v>
       </c>
@@ -1679,7 +1870,7 @@
         <v>3.3210000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>4.99</v>
       </c>
@@ -1704,8 +1895,14 @@
       <c r="H41" s="1">
         <v>3.948</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M41" s="4">
+        <v>6.9643331999999996</v>
+      </c>
+      <c r="N41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4.99</v>
       </c>
@@ -1730,8 +1927,11 @@
       <c r="H42" s="1">
         <v>2.3570000000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M42" s="4">
+        <v>2.83033331999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>4.99</v>
       </c>
@@ -1756,8 +1956,11 @@
       <c r="H43" s="1">
         <v>2.1560000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M43" s="4">
+        <v>0.50408971999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4.99</v>
       </c>
@@ -1782,8 +1985,11 @@
       <c r="H44" s="1">
         <v>2.7669999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M44" s="4">
+        <v>38.333333199999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>4.99</v>
       </c>
@@ -1808,8 +2014,11 @@
       <c r="H45" s="1">
         <v>3.8239999999999998</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M45" s="4">
+        <v>-4.8666666000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>4.99</v>
       </c>
@@ -1834,8 +2043,11 @@
       <c r="H46" s="1">
         <v>1.9730000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M46" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>4.99</v>
       </c>
@@ -1860,8 +2072,11 @@
       <c r="H47" s="1">
         <v>1.929</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M47" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>4.99</v>
       </c>
@@ -1886,8 +2101,11 @@
       <c r="H48" s="1">
         <v>2.181</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M48" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>4.99</v>
       </c>
@@ -1913,7 +2131,7 @@
         <v>2.4220000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>4.99</v>
       </c>
@@ -1938,8 +2156,14 @@
       <c r="H50" s="1">
         <v>2.7090000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M50" s="4">
+        <v>4.5653031999999998</v>
+      </c>
+      <c r="N50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>4.99</v>
       </c>
@@ -1964,8 +2188,11 @@
       <c r="H51" s="1">
         <v>3.2639999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M51" s="4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>4.99</v>
       </c>
@@ -1990,8 +2217,11 @@
       <c r="H52" s="1">
         <v>3.4969999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M52" s="4">
+        <v>-3.2647620000000002E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>4.99</v>
       </c>
@@ -2016,8 +2246,11 @@
       <c r="H53" s="1">
         <v>3.718</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M53" s="4">
+        <v>35.666666800000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>4.99</v>
       </c>
@@ -2042,8 +2275,11 @@
       <c r="H54" s="1">
         <v>1.9990000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M54" s="4">
+        <v>-4.8666666000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>4.99</v>
       </c>
@@ -2068,8 +2304,11 @@
       <c r="H55" s="1">
         <v>1.889</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M55" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>4.99</v>
       </c>
@@ -2094,8 +2333,11 @@
       <c r="H56" s="1">
         <v>1.6950000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M56" s="4">
+        <v>-0.47620109999999899</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>4.99</v>
       </c>
@@ -2120,8 +2362,11 @@
       <c r="H57" s="1">
         <v>2.6360000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M57" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>3.875</v>
       </c>
@@ -2150,7 +2395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>3.875</v>
       </c>
@@ -2175,8 +2420,14 @@
       <c r="H59" s="1">
         <v>1.649</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M59" s="4">
+        <v>7.3488331999999996</v>
+      </c>
+      <c r="N59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>3.875</v>
       </c>
@@ -2201,8 +2452,11 @@
       <c r="H60" s="1">
         <v>1.466</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M60" s="4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>3.875</v>
       </c>
@@ -2227,8 +2481,11 @@
       <c r="H61" s="1">
         <v>1.3360000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M61" s="4">
+        <v>0.53575491999999902</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>3.875</v>
       </c>
@@ -2253,8 +2510,11 @@
       <c r="H62" s="1">
         <v>0.98399999999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M62" s="4">
+        <v>37.353333199999902</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>3.875</v>
       </c>
@@ -2279,8 +2539,11 @@
       <c r="H63" s="1">
         <v>0.89200000000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M63" s="4">
+        <v>-5.3666666000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>3.875</v>
       </c>
@@ -2305,8 +2568,11 @@
       <c r="H64" s="1">
         <v>0.80700000000000005</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M64" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>3.875</v>
       </c>
@@ -2331,8 +2597,11 @@
       <c r="H65" s="1">
         <v>1.762</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M65" s="4">
+        <v>-1.4933334</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>3.875</v>
       </c>
@@ -2357,8 +2626,11 @@
       <c r="H66" s="1">
         <v>1.5660000000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M66" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>3.875</v>
       </c>
@@ -2384,7 +2656,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>3.875</v>
       </c>
@@ -2410,7 +2682,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>3.875</v>
       </c>
@@ -2436,7 +2708,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>3.875</v>
       </c>
@@ -2462,7 +2734,7 @@
         <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>3.875</v>
       </c>
@@ -2488,7 +2760,7 @@
         <v>1.885</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>3.875</v>
       </c>
@@ -2514,7 +2786,7 @@
         <v>1.635</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>3.875</v>
       </c>
@@ -2540,7 +2812,7 @@
         <v>1.4850000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>3.875</v>
       </c>
@@ -2566,7 +2838,7 @@
         <v>1.232</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>3.875</v>
       </c>
@@ -2592,7 +2864,7 @@
         <v>1.1559999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>3.875</v>
       </c>
@@ -2618,7 +2890,7 @@
         <v>1.004</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>3.875</v>
       </c>
@@ -2644,7 +2916,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>3.875</v>
       </c>
@@ -2670,189 +2942,189 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>3.875</v>
+        <v>4.67</v>
       </c>
       <c r="B79" s="1">
-        <v>3.7559999999999998</v>
+        <v>1.64</v>
       </c>
       <c r="C79" s="1">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="D79" s="2">
-        <v>296.75</v>
+        <v>296.34999999999997</v>
       </c>
       <c r="E79" s="2">
-        <v>303.25</v>
+        <v>298.14999999999998</v>
       </c>
       <c r="F79" s="3">
-        <v>148</v>
+        <v>245</v>
       </c>
       <c r="G79" s="3">
-        <v>383</v>
+        <v>72</v>
       </c>
       <c r="H79" s="1">
-        <v>0.53400000000000003</v>
+        <v>1.821</v>
       </c>
       <c r="I79" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>3.6739999999999999</v>
+        <v>4.67</v>
       </c>
       <c r="B80" s="1">
-        <v>3.952</v>
+        <v>1.2</v>
       </c>
       <c r="C80" s="1">
-        <v>0.104</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D80" s="2">
-        <v>296.95</v>
+        <v>296.14999999999998</v>
       </c>
       <c r="E80" s="2">
-        <v>304.34999999999997</v>
+        <v>297.75</v>
       </c>
       <c r="F80" s="3">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="G80" s="3">
-        <v>1112</v>
+        <v>62</v>
       </c>
       <c r="H80" s="1">
-        <v>0.19900000000000001</v>
+        <v>1.994</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>4.1559999999999997</v>
+        <v>4.67</v>
       </c>
       <c r="B81" s="1">
-        <v>4.7489999999999997</v>
+        <v>0.84</v>
       </c>
       <c r="C81" s="1">
-        <v>9.8000000000000004E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D81" s="2">
-        <v>296.75</v>
+        <v>296.25</v>
       </c>
       <c r="E81" s="2">
-        <v>304.04999999999995</v>
+        <v>296.64999999999998</v>
       </c>
       <c r="F81" s="3">
-        <v>394</v>
+        <v>142</v>
       </c>
       <c r="G81" s="3">
-        <v>197</v>
+        <v>54</v>
       </c>
       <c r="H81" s="1">
-        <v>0.95899999999999996</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>4.3959999999999999</v>
+        <v>4.67</v>
       </c>
       <c r="B82" s="1">
-        <v>4.2809999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="C82" s="1">
-        <v>0.10199999999999999</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D82" s="2">
-        <v>297.04999999999995</v>
+        <v>296.54999999999995</v>
       </c>
       <c r="E82" s="2">
-        <v>304.84999999999997</v>
+        <v>296.75</v>
       </c>
       <c r="F82" s="3">
-        <v>334</v>
+        <v>100</v>
       </c>
       <c r="G82" s="3">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="H82" s="1">
-        <v>1.2889999999999999</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>4.63</v>
+        <v>4.67</v>
       </c>
       <c r="B83" s="1">
-        <v>4.2229999999999999</v>
+        <v>2.16</v>
       </c>
       <c r="C83" s="1">
-        <v>0.10199999999999999</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D83" s="2">
-        <v>296.95</v>
+        <v>296.64999999999998</v>
       </c>
       <c r="E83" s="2">
-        <v>305.75</v>
+        <v>300.14999999999998</v>
       </c>
       <c r="F83" s="3">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="G83" s="3">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="H83" s="1">
-        <v>1.514</v>
+        <v>1.5669999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>4.91</v>
+        <v>4.67</v>
       </c>
       <c r="B84" s="1">
-        <v>4.1260000000000003</v>
+        <v>2.72</v>
       </c>
       <c r="C84" s="1">
-        <v>0.108</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="D84" s="2">
-        <v>297.04999999999995</v>
+        <v>296.45</v>
       </c>
       <c r="E84" s="2">
-        <v>306.64999999999998</v>
+        <v>301.34999999999997</v>
       </c>
       <c r="F84" s="3">
-        <v>227</v>
+        <v>270</v>
       </c>
       <c r="G84" s="3">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H84" s="1">
-        <v>1.8080000000000001</v>
+        <v>1.4970000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>5.07</v>
+        <v>4.67</v>
       </c>
       <c r="B85" s="1">
-        <v>4.0490000000000004</v>
+        <v>3.24</v>
       </c>
       <c r="C85" s="1">
-        <v>0.108</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="D85" s="2">
-        <v>296.95</v>
+        <v>296.14999999999998</v>
       </c>
       <c r="E85" s="2">
-        <v>307.04999999999995</v>
+        <v>303.14999999999998</v>
       </c>
       <c r="F85" s="3">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="G85" s="3">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="H85" s="1">
-        <v>2.1179999999999999</v>
+        <v>1.427</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -2860,28 +3132,25 @@
         <v>4.67</v>
       </c>
       <c r="B86" s="1">
-        <v>1.64</v>
+        <v>3.76</v>
       </c>
       <c r="C86" s="1">
-        <v>0.04</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D86" s="2">
         <v>296.34999999999997</v>
       </c>
       <c r="E86" s="2">
-        <v>298.14999999999998</v>
+        <v>304.14999999999998</v>
       </c>
       <c r="F86" s="3">
-        <v>245</v>
+        <v>302</v>
       </c>
       <c r="G86" s="3">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="H86" s="1">
-        <v>1.821</v>
-      </c>
-      <c r="I86" t="s">
-        <v>14</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -2889,25 +3158,25 @@
         <v>4.67</v>
       </c>
       <c r="B87" s="1">
-        <v>1.2</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="C87" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0.108</v>
       </c>
       <c r="D87" s="2">
-        <v>296.14999999999998</v>
+        <v>296.64999999999998</v>
       </c>
       <c r="E87" s="2">
-        <v>297.75</v>
+        <v>306.14999999999998</v>
       </c>
       <c r="F87" s="3">
-        <v>204</v>
+        <v>317</v>
       </c>
       <c r="G87" s="3">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="H87" s="1">
-        <v>1.994</v>
+        <v>1.2849999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -2915,25 +3184,25 @@
         <v>4.67</v>
       </c>
       <c r="B88" s="1">
-        <v>0.84</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="C88" s="1">
-        <v>1.4E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D88" s="2">
         <v>296.25</v>
       </c>
       <c r="E88" s="2">
-        <v>296.64999999999998</v>
+        <v>297.04999999999995</v>
       </c>
       <c r="F88" s="3">
-        <v>142</v>
+        <v>96.7</v>
       </c>
       <c r="G88" s="3">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H88" s="1">
-        <v>2.2999999999999998</v>
+        <v>2.4980000000000002</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -2941,25 +3210,25 @@
         <v>4.67</v>
       </c>
       <c r="B89" s="1">
-        <v>0.71199999999999997</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="C89" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D89" s="2">
         <v>296.54999999999995</v>
       </c>
       <c r="E89" s="2">
-        <v>296.75</v>
+        <v>297.84999999999997</v>
       </c>
       <c r="F89" s="3">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G89" s="3">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H89" s="1">
-        <v>2.44</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -2967,25 +3236,25 @@
         <v>4.67</v>
       </c>
       <c r="B90" s="1">
-        <v>2.16</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="C90" s="1">
-        <v>5.3999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D90" s="2">
-        <v>296.64999999999998</v>
+        <v>296.45</v>
       </c>
       <c r="E90" s="2">
-        <v>300.14999999999998</v>
+        <v>297.95</v>
       </c>
       <c r="F90" s="3">
-        <v>250</v>
+        <v>95</v>
       </c>
       <c r="G90" s="3">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="H90" s="1">
-        <v>1.5669999999999999</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -2993,25 +3262,25 @@
         <v>4.67</v>
       </c>
       <c r="B91" s="1">
-        <v>2.72</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="C91" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D91" s="2">
-        <v>296.45</v>
+        <v>296.14999999999998</v>
       </c>
       <c r="E91" s="2">
-        <v>301.34999999999997</v>
+        <v>297.64999999999998</v>
       </c>
       <c r="F91" s="3">
-        <v>270</v>
+        <v>95</v>
       </c>
       <c r="G91" s="3">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="H91" s="1">
-        <v>1.4970000000000001</v>
+        <v>2.637</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3019,25 +3288,25 @@
         <v>4.67</v>
       </c>
       <c r="B92" s="1">
-        <v>3.24</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="C92" s="1">
-        <v>8.1000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D92" s="2">
         <v>296.14999999999998</v>
       </c>
       <c r="E92" s="2">
-        <v>303.14999999999998</v>
+        <v>297.75</v>
       </c>
       <c r="F92" s="3">
-        <v>290</v>
+        <v>94</v>
       </c>
       <c r="G92" s="3">
-        <v>93</v>
+        <v>23</v>
       </c>
       <c r="H92" s="1">
-        <v>1.427</v>
+        <v>2.7149999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3045,25 +3314,28 @@
         <v>4.67</v>
       </c>
       <c r="B93" s="1">
-        <v>3.76</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="C93" s="1">
-        <v>9.4E-2</v>
+        <v>0</v>
       </c>
       <c r="D93" s="2">
-        <v>296.34999999999997</v>
+        <v>301.84999999999997</v>
       </c>
       <c r="E93" s="2">
-        <v>304.14999999999998</v>
+        <v>303.04999999999995</v>
       </c>
       <c r="F93" s="3">
-        <v>302</v>
+        <v>100</v>
       </c>
       <c r="G93" s="3">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="H93" s="1">
-        <v>1.38</v>
+        <v>2.6</v>
+      </c>
+      <c r="I93" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -3071,25 +3343,25 @@
         <v>4.67</v>
       </c>
       <c r="B94" s="1">
-        <v>4.4400000000000004</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="C94" s="1">
-        <v>0.108</v>
+        <v>2E-3</v>
       </c>
       <c r="D94" s="2">
-        <v>296.64999999999998</v>
+        <v>302.25</v>
       </c>
       <c r="E94" s="2">
-        <v>306.14999999999998</v>
+        <v>303.45</v>
       </c>
       <c r="F94" s="3">
-        <v>317</v>
+        <v>98</v>
       </c>
       <c r="G94" s="3">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="H94" s="1">
-        <v>1.2849999999999999</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -3097,25 +3369,25 @@
         <v>4.67</v>
       </c>
       <c r="B95" s="1">
-        <v>0.66400000000000003</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="C95" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D95" s="2">
-        <v>296.25</v>
+        <v>303.54999999999995</v>
       </c>
       <c r="E95" s="2">
-        <v>297.04999999999995</v>
+        <v>305.64999999999998</v>
       </c>
       <c r="F95" s="3">
-        <v>96.7</v>
+        <v>101</v>
       </c>
       <c r="G95" s="3">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H95" s="1">
-        <v>2.4980000000000002</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3123,25 +3395,25 @@
         <v>4.67</v>
       </c>
       <c r="B96" s="1">
-        <v>0.64800000000000002</v>
+        <v>0.872</v>
       </c>
       <c r="C96" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D96" s="2">
-        <v>296.54999999999995</v>
+        <v>303.75</v>
       </c>
       <c r="E96" s="2">
-        <v>297.84999999999997</v>
+        <v>305.95</v>
       </c>
       <c r="F96" s="3">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="G96" s="3">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="H96" s="1">
-        <v>2.56</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3149,25 +3421,25 @@
         <v>4.67</v>
       </c>
       <c r="B97" s="1">
-        <v>0.61599999999999999</v>
+        <v>1.22</v>
       </c>
       <c r="C97" s="1">
-        <v>2E-3</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D97" s="2">
-        <v>296.45</v>
+        <v>304.14999999999998</v>
       </c>
       <c r="E97" s="2">
-        <v>297.95</v>
+        <v>306.45</v>
       </c>
       <c r="F97" s="3">
-        <v>95</v>
+        <v>210</v>
       </c>
       <c r="G97" s="3">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="H97" s="1">
-        <v>2.6</v>
+        <v>1.956</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3175,25 +3447,25 @@
         <v>4.67</v>
       </c>
       <c r="B98" s="1">
-        <v>0.60799999999999998</v>
+        <v>1.655</v>
       </c>
       <c r="C98" s="1">
-        <v>2E-3</v>
+        <v>0.04</v>
       </c>
       <c r="D98" s="2">
-        <v>296.14999999999998</v>
+        <v>304.64999999999998</v>
       </c>
       <c r="E98" s="2">
-        <v>297.64999999999998</v>
+        <v>307.75</v>
       </c>
       <c r="F98" s="3">
-        <v>95</v>
+        <v>198</v>
       </c>
       <c r="G98" s="3">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="H98" s="1">
-        <v>2.637</v>
+        <v>1.7689999999999999</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -3201,25 +3473,25 @@
         <v>4.67</v>
       </c>
       <c r="B99" s="1">
-        <v>0.58399999999999996</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="C99" s="1">
-        <v>0</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D99" s="2">
-        <v>296.14999999999998</v>
+        <v>304.54999999999995</v>
       </c>
       <c r="E99" s="2">
-        <v>297.75</v>
+        <v>308.14999999999998</v>
       </c>
       <c r="F99" s="3">
-        <v>94</v>
+        <v>254</v>
       </c>
       <c r="G99" s="3">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="H99" s="1">
-        <v>2.7149999999999999</v>
+        <v>1.512</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -3227,28 +3499,25 @@
         <v>4.67</v>
       </c>
       <c r="B100" s="1">
-        <v>0.60799999999999998</v>
+        <v>2.72</v>
       </c>
       <c r="C100" s="1">
-        <v>0</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D100" s="2">
-        <v>301.84999999999997</v>
+        <v>305.45</v>
       </c>
       <c r="E100" s="2">
-        <v>303.04999999999995</v>
+        <v>309.64999999999998</v>
       </c>
       <c r="F100" s="3">
-        <v>100</v>
+        <v>284</v>
       </c>
       <c r="G100" s="3">
-        <v>24</v>
-      </c>
-      <c r="H100" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="I100" t="s">
-        <v>15</v>
+        <v>87</v>
+      </c>
+      <c r="H100">
+        <v>1.427</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -3256,25 +3525,25 @@
         <v>4.67</v>
       </c>
       <c r="B101" s="1">
-        <v>0.63200000000000001</v>
+        <v>3.24</v>
       </c>
       <c r="C101" s="1">
-        <v>2E-3</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D101" s="2">
-        <v>302.25</v>
+        <v>305.64999999999998</v>
       </c>
       <c r="E101" s="2">
-        <v>303.45</v>
+        <v>311.64999999999998</v>
       </c>
       <c r="F101" s="3">
-        <v>98</v>
+        <v>283</v>
       </c>
       <c r="G101" s="3">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="H101" s="1">
-        <v>2.6</v>
+        <v>1.4530000000000001</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -3282,25 +3551,25 @@
         <v>4.67</v>
       </c>
       <c r="B102" s="1">
-        <v>0.72799999999999998</v>
+        <v>3.76</v>
       </c>
       <c r="C102" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D102" s="2">
-        <v>303.54999999999995</v>
+        <v>305.75</v>
       </c>
       <c r="E102" s="2">
-        <v>305.64999999999998</v>
+        <v>312.25</v>
       </c>
       <c r="F102" s="3">
-        <v>101</v>
+        <v>292</v>
       </c>
       <c r="G102" s="3">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="H102" s="1">
-        <v>2.4500000000000002</v>
+        <v>1.4339999999999999</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -3308,25 +3577,25 @@
         <v>4.67</v>
       </c>
       <c r="B103" s="1">
-        <v>0.872</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C103" s="1">
-        <v>1.4E-2</v>
+        <v>0.108</v>
       </c>
       <c r="D103" s="2">
-        <v>303.75</v>
+        <v>305.64999999999998</v>
       </c>
       <c r="E103" s="2">
-        <v>305.95</v>
+        <v>313.64999999999998</v>
       </c>
       <c r="F103" s="3">
-        <v>150</v>
+        <v>311</v>
       </c>
       <c r="G103" s="3">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="H103" s="1">
-        <v>2.1800000000000002</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -3334,25 +3603,28 @@
         <v>4.67</v>
       </c>
       <c r="B104" s="1">
-        <v>1.22</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="C104" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D104" s="2">
-        <v>304.14999999999998</v>
+        <v>314.04999999999995</v>
       </c>
       <c r="E104" s="2">
-        <v>306.45</v>
+        <v>316.25</v>
       </c>
       <c r="F104" s="3">
-        <v>210</v>
+        <v>98</v>
       </c>
       <c r="G104" s="3">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="H104" s="1">
-        <v>1.956</v>
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="I104" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -3360,25 +3632,25 @@
         <v>4.67</v>
       </c>
       <c r="B105" s="1">
-        <v>1.655</v>
+        <v>0.6</v>
       </c>
       <c r="C105" s="1">
-        <v>0.04</v>
+        <v>1E-3</v>
       </c>
       <c r="D105" s="2">
-        <v>304.64999999999998</v>
+        <v>314.34999999999997</v>
       </c>
       <c r="E105" s="2">
-        <v>307.75</v>
+        <v>316.84999999999997</v>
       </c>
       <c r="F105" s="3">
-        <v>198</v>
+        <v>97</v>
       </c>
       <c r="G105" s="3">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="H105" s="1">
-        <v>1.7689999999999999</v>
+        <v>2.6930000000000001</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,25 +3658,25 @@
         <v>4.67</v>
       </c>
       <c r="B106" s="1">
-        <v>2.1800000000000002</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="C106" s="1">
-        <v>5.3999999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D106" s="2">
-        <v>304.54999999999995</v>
+        <v>314.95</v>
       </c>
       <c r="E106" s="2">
-        <v>308.14999999999998</v>
+        <v>317.45</v>
       </c>
       <c r="F106" s="3">
-        <v>254</v>
+        <v>95</v>
       </c>
       <c r="G106" s="3">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="H106" s="1">
-        <v>1.512</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3412,25 +3684,25 @@
         <v>4.67</v>
       </c>
       <c r="B107" s="1">
-        <v>2.72</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="C107" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D107" s="2">
-        <v>305.45</v>
+        <v>315.25</v>
       </c>
       <c r="E107" s="2">
-        <v>309.64999999999998</v>
+        <v>317.95</v>
       </c>
       <c r="F107" s="3">
-        <v>284</v>
+        <v>95</v>
       </c>
       <c r="G107" s="3">
-        <v>87</v>
-      </c>
-      <c r="H107">
-        <v>1.427</v>
+        <v>36</v>
+      </c>
+      <c r="H107" s="1">
+        <v>2.56</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -3438,25 +3710,25 @@
         <v>4.67</v>
       </c>
       <c r="B108" s="1">
-        <v>3.24</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="C108" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D108" s="2">
-        <v>305.64999999999998</v>
+        <v>315.95</v>
       </c>
       <c r="E108" s="2">
-        <v>311.64999999999998</v>
+        <v>318.54999999999995</v>
       </c>
       <c r="F108" s="3">
-        <v>283</v>
+        <v>97</v>
       </c>
       <c r="G108" s="3">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="H108" s="1">
-        <v>1.4530000000000001</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -3464,25 +3736,25 @@
         <v>4.67</v>
       </c>
       <c r="B109" s="1">
-        <v>3.76</v>
+        <v>0.84</v>
       </c>
       <c r="C109" s="1">
-        <v>9.4E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D109" s="2">
-        <v>305.75</v>
+        <v>315.95</v>
       </c>
       <c r="E109" s="2">
-        <v>312.25</v>
+        <v>318.64999999999998</v>
       </c>
       <c r="F109" s="3">
-        <v>292</v>
+        <v>143</v>
       </c>
       <c r="G109" s="3">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="H109" s="1">
-        <v>1.4339999999999999</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -3490,25 +3762,25 @@
         <v>4.67</v>
       </c>
       <c r="B110" s="1">
-        <v>4.4000000000000004</v>
+        <v>1.2</v>
       </c>
       <c r="C110" s="1">
-        <v>0.108</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D110" s="2">
-        <v>305.64999999999998</v>
+        <v>316.45</v>
       </c>
       <c r="E110" s="2">
-        <v>313.64999999999998</v>
+        <v>319.25</v>
       </c>
       <c r="F110" s="3">
-        <v>311</v>
+        <v>197</v>
       </c>
       <c r="G110" s="3">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="H110" s="1">
-        <v>1.34</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -3516,28 +3788,25 @@
         <v>4.67</v>
       </c>
       <c r="B111" s="1">
-        <v>0.59199999999999997</v>
+        <v>1.64</v>
       </c>
       <c r="C111" s="1">
-        <v>0</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D111" s="2">
-        <v>314.04999999999995</v>
+        <v>317.34999999999997</v>
       </c>
       <c r="E111" s="2">
-        <v>316.25</v>
+        <v>320.34999999999997</v>
       </c>
       <c r="F111" s="3">
-        <v>98</v>
+        <v>190</v>
       </c>
       <c r="G111" s="3">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="H111" s="1">
-        <v>2.7349999999999999</v>
-      </c>
-      <c r="I111" t="s">
-        <v>16</v>
+        <v>1.819</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -3545,25 +3814,25 @@
         <v>4.67</v>
       </c>
       <c r="B112" s="1">
-        <v>0.6</v>
+        <v>2.1539999999999999</v>
       </c>
       <c r="C112" s="1">
-        <v>1E-3</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="D112" s="2">
-        <v>314.34999999999997</v>
+        <v>316.95</v>
       </c>
       <c r="E112" s="2">
-        <v>316.84999999999997</v>
+        <v>321.04999999999995</v>
       </c>
       <c r="F112" s="3">
-        <v>97</v>
+        <v>233</v>
       </c>
       <c r="G112" s="3">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="H112" s="1">
-        <v>2.6930000000000001</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -3571,25 +3840,25 @@
         <v>4.67</v>
       </c>
       <c r="B113" s="1">
-        <v>0.61599999999999999</v>
+        <v>2.661</v>
       </c>
       <c r="C113" s="1">
-        <v>2E-3</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D113" s="2">
-        <v>314.95</v>
+        <v>316.95</v>
       </c>
       <c r="E113" s="2">
-        <v>317.45</v>
+        <v>321.64999999999998</v>
       </c>
       <c r="F113" s="3">
-        <v>95</v>
+        <v>252</v>
       </c>
       <c r="G113" s="3">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="H113" s="1">
-        <v>2.6</v>
+        <v>1.581</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -3597,25 +3866,25 @@
         <v>4.67</v>
       </c>
       <c r="B114" s="1">
-        <v>0.65600000000000003</v>
+        <v>3.1629999999999998</v>
       </c>
       <c r="C114" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D114" s="2">
-        <v>315.25</v>
+        <v>317.34999999999997</v>
       </c>
       <c r="E114" s="2">
-        <v>317.95</v>
+        <v>323.14999999999998</v>
       </c>
       <c r="F114" s="3">
-        <v>95</v>
+        <v>251</v>
       </c>
       <c r="G114" s="3">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="H114" s="1">
-        <v>2.56</v>
+        <v>1.6060000000000001</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -3623,25 +3892,25 @@
         <v>4.67</v>
       </c>
       <c r="B115" s="1">
-        <v>0.70399999999999996</v>
+        <v>3.7320000000000002</v>
       </c>
       <c r="C115" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D115" s="2">
-        <v>315.95</v>
+        <v>317.25</v>
       </c>
       <c r="E115" s="2">
-        <v>318.54999999999995</v>
+        <v>323.95</v>
       </c>
       <c r="F115" s="3">
-        <v>97</v>
+        <v>284</v>
       </c>
       <c r="G115" s="3">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="H115" s="1">
-        <v>2.4500000000000002</v>
+        <v>1.4570000000000001</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -3649,25 +3918,25 @@
         <v>4.67</v>
       </c>
       <c r="B116" s="1">
-        <v>0.84</v>
+        <v>4.3259999999999996</v>
       </c>
       <c r="C116" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D116" s="2">
-        <v>315.95</v>
+        <v>317.14999999999998</v>
       </c>
       <c r="E116" s="2">
-        <v>318.64999999999998</v>
+        <v>325.75</v>
       </c>
       <c r="F116" s="3">
-        <v>143</v>
+        <v>295</v>
       </c>
       <c r="G116" s="3">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="H116" s="1">
-        <v>2.21</v>
+        <v>1.41</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -3675,25 +3944,28 @@
         <v>4.67</v>
       </c>
       <c r="B117" s="1">
-        <v>1.2</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C117" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D117" s="2">
-        <v>316.45</v>
+        <v>322.95</v>
       </c>
       <c r="E117" s="2">
-        <v>319.25</v>
+        <v>324.14999999999998</v>
       </c>
       <c r="F117" s="3">
-        <v>197</v>
+        <v>89</v>
       </c>
       <c r="G117" s="3">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="H117" s="1">
-        <v>2.0099999999999998</v>
+        <v>2.8769999999999998</v>
+      </c>
+      <c r="I117" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -3701,25 +3973,25 @@
         <v>4.67</v>
       </c>
       <c r="B118" s="1">
-        <v>1.64</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="C118" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D118" s="2">
-        <v>317.34999999999997</v>
+        <v>322.95</v>
       </c>
       <c r="E118" s="2">
-        <v>320.34999999999997</v>
+        <v>325.14999999999998</v>
       </c>
       <c r="F118" s="3">
-        <v>190</v>
+        <v>92</v>
       </c>
       <c r="G118" s="3">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="H118" s="1">
-        <v>1.819</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -3727,25 +3999,25 @@
         <v>4.67</v>
       </c>
       <c r="B119" s="1">
-        <v>2.1539999999999999</v>
+        <v>0.6</v>
       </c>
       <c r="C119" s="1">
-        <v>5.6000000000000001E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D119" s="2">
-        <v>316.95</v>
+        <v>323.14999999999998</v>
       </c>
       <c r="E119" s="2">
-        <v>321.04999999999995</v>
+        <v>325.75</v>
       </c>
       <c r="F119" s="3">
-        <v>233</v>
+        <v>92</v>
       </c>
       <c r="G119" s="3">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="H119" s="1">
-        <v>1.625</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -3753,25 +4025,25 @@
         <v>4.67</v>
       </c>
       <c r="B120" s="1">
-        <v>2.661</v>
+        <v>0.64</v>
       </c>
       <c r="C120" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D120" s="2">
-        <v>316.95</v>
+        <v>323.45</v>
       </c>
       <c r="E120" s="2">
-        <v>321.64999999999998</v>
+        <v>325.64999999999998</v>
       </c>
       <c r="F120" s="3">
-        <v>252</v>
+        <v>92</v>
       </c>
       <c r="G120" s="3">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="H120" s="1">
-        <v>1.581</v>
+        <v>2.6829999999999998</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -3779,25 +4051,25 @@
         <v>4.67</v>
       </c>
       <c r="B121" s="1">
-        <v>3.1629999999999998</v>
+        <v>0.68</v>
       </c>
       <c r="C121" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D121" s="2">
-        <v>317.34999999999997</v>
+        <v>323.75</v>
       </c>
       <c r="E121" s="2">
-        <v>323.14999999999998</v>
+        <v>325.84999999999997</v>
       </c>
       <c r="F121" s="3">
-        <v>251</v>
+        <v>92</v>
       </c>
       <c r="G121" s="3">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="H121" s="1">
-        <v>1.6060000000000001</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -3805,25 +4077,25 @@
         <v>4.67</v>
       </c>
       <c r="B122" s="1">
-        <v>3.7320000000000002</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="C122" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D122" s="2">
-        <v>317.25</v>
+        <v>323.14999999999998</v>
       </c>
       <c r="E122" s="2">
-        <v>323.95</v>
+        <v>326.54999999999995</v>
       </c>
       <c r="F122" s="3">
-        <v>284</v>
+        <v>139</v>
       </c>
       <c r="G122" s="3">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="H122" s="1">
-        <v>1.4570000000000001</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -3831,25 +4103,25 @@
         <v>4.67</v>
       </c>
       <c r="B123" s="1">
-        <v>4.3259999999999996</v>
+        <v>1.016</v>
       </c>
       <c r="C123" s="1">
-        <v>1.0900000000000001</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D123" s="2">
-        <v>317.14999999999998</v>
+        <v>323.34999999999997</v>
       </c>
       <c r="E123" s="2">
-        <v>325.75</v>
+        <v>325.84999999999997</v>
       </c>
       <c r="F123" s="3">
-        <v>295</v>
+        <v>188</v>
       </c>
       <c r="G123" s="3">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="H123" s="1">
-        <v>1.41</v>
+        <v>2.0150000000000001</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -3857,28 +4129,25 @@
         <v>4.67</v>
       </c>
       <c r="B124" s="1">
-        <v>0.56000000000000005</v>
+        <v>1.1870000000000001</v>
       </c>
       <c r="C124" s="1">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D124" s="2">
-        <v>322.95</v>
+        <v>324.04999999999995</v>
       </c>
       <c r="E124" s="2">
-        <v>324.14999999999998</v>
+        <v>326.45</v>
       </c>
       <c r="F124" s="3">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="G124" s="3">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="H124" s="1">
-        <v>2.8769999999999998</v>
-      </c>
-      <c r="I124" t="s">
-        <v>17</v>
+        <v>1.9670000000000001</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -3886,25 +4155,25 @@
         <v>4.67</v>
       </c>
       <c r="B125" s="1">
-        <v>0.58399999999999996</v>
+        <v>1.6519999999999999</v>
       </c>
       <c r="C125" s="1">
-        <v>2E-3</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D125" s="2">
-        <v>322.95</v>
+        <v>324.14999999999998</v>
       </c>
       <c r="E125" s="2">
-        <v>325.14999999999998</v>
+        <v>327.04999999999995</v>
       </c>
       <c r="F125" s="3">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="G125" s="3">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="H125" s="1">
-        <v>2.85</v>
+        <v>1.772</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -3912,25 +4181,25 @@
         <v>4.67</v>
       </c>
       <c r="B126" s="1">
-        <v>0.6</v>
+        <v>2.1379999999999999</v>
       </c>
       <c r="C126" s="1">
-        <v>2E-3</v>
+        <v>5.5E-2</v>
       </c>
       <c r="D126" s="2">
-        <v>323.14999999999998</v>
+        <v>324.04999999999995</v>
       </c>
       <c r="E126" s="2">
-        <v>325.75</v>
+        <v>327.45</v>
       </c>
       <c r="F126" s="3">
-        <v>92</v>
+        <v>224</v>
       </c>
       <c r="G126" s="3">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="H126" s="1">
-        <v>2.77</v>
+        <v>1.696</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -3938,25 +4207,25 @@
         <v>4.67</v>
       </c>
       <c r="B127" s="1">
-        <v>0.64</v>
+        <v>2.6560000000000001</v>
       </c>
       <c r="C127" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D127" s="2">
-        <v>323.45</v>
+        <v>324.04999999999995</v>
       </c>
       <c r="E127" s="2">
-        <v>325.64999999999998</v>
+        <v>328.65</v>
       </c>
       <c r="F127" s="3">
-        <v>92</v>
+        <v>248</v>
       </c>
       <c r="G127" s="3">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="H127" s="1">
-        <v>2.6829999999999998</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -3964,25 +4233,25 @@
         <v>4.67</v>
       </c>
       <c r="B128" s="1">
-        <v>0.68</v>
+        <v>3.21</v>
       </c>
       <c r="C128" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D128" s="2">
-        <v>323.75</v>
+        <v>324.45</v>
       </c>
       <c r="E128" s="2">
-        <v>325.84999999999997</v>
+        <v>329.84999999999997</v>
       </c>
       <c r="F128" s="3">
-        <v>92</v>
+        <v>265</v>
       </c>
       <c r="G128" s="3">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="H128" s="1">
-        <v>2.58</v>
+        <v>1.536</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -3990,25 +4259,25 @@
         <v>4.67</v>
       </c>
       <c r="B129" s="1">
-        <v>0.82399999999999995</v>
+        <v>3.7549999999999999</v>
       </c>
       <c r="C129" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D129" s="2">
-        <v>323.14999999999998</v>
+        <v>324.34999999999997</v>
       </c>
       <c r="E129" s="2">
-        <v>326.54999999999995</v>
+        <v>330.54999999999995</v>
       </c>
       <c r="F129" s="3">
-        <v>139</v>
+        <v>282</v>
       </c>
       <c r="G129" s="3">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="H129" s="1">
-        <v>2.29</v>
+        <v>1.484</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4016,25 +4285,25 @@
         <v>4.67</v>
       </c>
       <c r="B130" s="1">
-        <v>1.016</v>
+        <v>4.3970000000000002</v>
       </c>
       <c r="C130" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.109</v>
       </c>
       <c r="D130" s="2">
-        <v>323.34999999999997</v>
+        <v>324.54999999999995</v>
       </c>
       <c r="E130" s="2">
-        <v>325.84999999999997</v>
+        <v>331.84999999999997</v>
       </c>
       <c r="F130" s="3">
-        <v>188</v>
+        <v>307</v>
       </c>
       <c r="G130" s="3">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="H130" s="1">
-        <v>2.0150000000000001</v>
+        <v>1.3580000000000001</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -4042,25 +4311,28 @@
         <v>4.67</v>
       </c>
       <c r="B131" s="1">
-        <v>1.1870000000000001</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="C131" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D131" s="2">
-        <v>324.04999999999995</v>
+        <v>335.95</v>
       </c>
       <c r="E131" s="2">
-        <v>326.45</v>
+        <v>338.25</v>
       </c>
       <c r="F131" s="3">
-        <v>201</v>
+        <v>81</v>
       </c>
       <c r="G131" s="3">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="H131" s="1">
-        <v>1.9670000000000001</v>
+        <v>2.996</v>
+      </c>
+      <c r="I131" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -4068,25 +4340,25 @@
         <v>4.67</v>
       </c>
       <c r="B132" s="1">
-        <v>1.6519999999999999</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="C132" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D132" s="2">
-        <v>324.14999999999998</v>
+        <v>333.95</v>
       </c>
       <c r="E132" s="2">
-        <v>327.04999999999995</v>
+        <v>335.45</v>
       </c>
       <c r="F132" s="3">
-        <v>197</v>
+        <v>90</v>
       </c>
       <c r="G132" s="3">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="H132" s="1">
-        <v>1.772</v>
+        <v>2.8639999999999999</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4094,25 +4366,25 @@
         <v>4.67</v>
       </c>
       <c r="B133" s="1">
-        <v>2.1379999999999999</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C133" s="1">
-        <v>5.5E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="D133" s="2">
-        <v>324.04999999999995</v>
+        <v>332.95</v>
       </c>
       <c r="E133" s="2">
-        <v>327.45</v>
+        <v>334.65</v>
       </c>
       <c r="F133" s="3">
-        <v>224</v>
+        <v>92</v>
       </c>
       <c r="G133" s="3">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="H133" s="1">
-        <v>1.696</v>
+        <v>2.84</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -4120,25 +4392,25 @@
         <v>4.67</v>
       </c>
       <c r="B134" s="1">
-        <v>2.6560000000000001</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="C134" s="1">
-        <v>6.8000000000000005E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D134" s="2">
-        <v>324.04999999999995</v>
+        <v>332.75</v>
       </c>
       <c r="E134" s="2">
-        <v>328.65</v>
+        <v>334.34999999999997</v>
       </c>
       <c r="F134" s="3">
-        <v>248</v>
+        <v>92</v>
       </c>
       <c r="G134" s="3">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="H134" s="1">
-        <v>1.6</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -4146,25 +4418,25 @@
         <v>4.67</v>
       </c>
       <c r="B135" s="1">
-        <v>3.21</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="C135" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D135" s="2">
-        <v>324.45</v>
+        <v>332.25</v>
       </c>
       <c r="E135" s="2">
-        <v>329.84999999999997</v>
+        <v>334.15</v>
       </c>
       <c r="F135" s="3">
-        <v>265</v>
+        <v>91</v>
       </c>
       <c r="G135" s="3">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H135" s="1">
-        <v>1.536</v>
+        <v>2.6379999999999999</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -4172,25 +4444,25 @@
         <v>4.67</v>
       </c>
       <c r="B136" s="1">
-        <v>3.7549999999999999</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="C136" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D136" s="2">
-        <v>324.34999999999997</v>
+        <v>332.04999999999995</v>
       </c>
       <c r="E136" s="2">
-        <v>330.54999999999995</v>
+        <v>333.95</v>
       </c>
       <c r="F136" s="3">
-        <v>282</v>
+        <v>135</v>
       </c>
       <c r="G136" s="3">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="H136" s="1">
-        <v>1.484</v>
+        <v>2.3340000000000001</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -4198,25 +4470,25 @@
         <v>4.67</v>
       </c>
       <c r="B137" s="1">
-        <v>4.3970000000000002</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="C137" s="1">
-        <v>0.109</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D137" s="2">
-        <v>324.54999999999995</v>
+        <v>331.95</v>
       </c>
       <c r="E137" s="2">
-        <v>331.84999999999997</v>
+        <v>334.15</v>
       </c>
       <c r="F137" s="3">
-        <v>307</v>
+        <v>171</v>
       </c>
       <c r="G137" s="3">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="H137" s="1">
-        <v>1.3580000000000001</v>
+        <v>2.226</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -4224,28 +4496,25 @@
         <v>4.67</v>
       </c>
       <c r="B138" s="1">
-        <v>0.53600000000000003</v>
+        <v>1.1870000000000001</v>
       </c>
       <c r="C138" s="1">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D138" s="2">
-        <v>335.95</v>
+        <v>332.04999999999995</v>
       </c>
       <c r="E138" s="2">
-        <v>338.25</v>
+        <v>334.34999999999997</v>
       </c>
       <c r="F138" s="3">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="G138" s="3">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="H138" s="1">
-        <v>2.996</v>
-      </c>
-      <c r="I138" t="s">
-        <v>18</v>
+        <v>2.0459999999999998</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -4253,25 +4522,25 @@
         <v>4.67</v>
       </c>
       <c r="B139" s="1">
-        <v>0.56799999999999995</v>
+        <v>1.6167</v>
       </c>
       <c r="C139" s="1">
-        <v>2E-3</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D139" s="2">
-        <v>333.95</v>
+        <v>331.65</v>
       </c>
       <c r="E139" s="2">
-        <v>335.45</v>
+        <v>334.34999999999997</v>
       </c>
       <c r="F139" s="3">
-        <v>90</v>
+        <v>204</v>
       </c>
       <c r="G139" s="3">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="H139" s="1">
-        <v>2.8639999999999999</v>
+        <v>1.9570000000000001</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -4279,25 +4548,25 @@
         <v>4.67</v>
       </c>
       <c r="B140" s="1">
-        <v>0.57599999999999996</v>
+        <v>2.1019999999999999</v>
       </c>
       <c r="C140" s="1">
-        <v>2E-3</v>
+        <v>5.5E-2</v>
       </c>
       <c r="D140" s="2">
-        <v>332.95</v>
+        <v>331.95</v>
       </c>
       <c r="E140" s="2">
-        <v>334.65</v>
+        <v>334.34999999999997</v>
       </c>
       <c r="F140" s="3">
-        <v>92</v>
+        <v>210</v>
       </c>
       <c r="G140" s="3">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="H140" s="1">
-        <v>2.84</v>
+        <v>1.8220000000000001</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -4305,25 +4574,25 @@
         <v>4.67</v>
       </c>
       <c r="B141" s="1">
-        <v>0.61599999999999999</v>
+        <v>2.621</v>
       </c>
       <c r="C141" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="D141" s="2">
-        <v>332.75</v>
+        <v>331.45</v>
       </c>
       <c r="E141" s="2">
-        <v>334.34999999999997</v>
+        <v>335.34999999999997</v>
       </c>
       <c r="F141" s="3">
-        <v>92</v>
+        <v>232</v>
       </c>
       <c r="G141" s="3">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="H141" s="1">
-        <v>2.74</v>
+        <v>1.7070000000000001</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -4331,25 +4600,25 @@
         <v>4.67</v>
       </c>
       <c r="B142" s="1">
-        <v>0.67200000000000004</v>
+        <v>3.1579999999999999</v>
       </c>
       <c r="C142" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D142" s="2">
-        <v>332.25</v>
+        <v>331.75</v>
       </c>
       <c r="E142" s="2">
-        <v>334.15</v>
+        <v>336.34999999999997</v>
       </c>
       <c r="F142" s="3">
-        <v>91</v>
+        <v>253</v>
       </c>
       <c r="G142" s="3">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="H142" s="1">
-        <v>2.6379999999999999</v>
+        <v>1.609</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -4357,25 +4626,25 @@
         <v>4.67</v>
       </c>
       <c r="B143" s="1">
-        <v>0.81599999999999995</v>
+        <v>3.6949999999999998</v>
       </c>
       <c r="C143" s="1">
-        <v>1.4E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D143" s="2">
-        <v>332.04999999999995</v>
+        <v>331.84999999999997</v>
       </c>
       <c r="E143" s="2">
-        <v>333.95</v>
+        <v>337.75</v>
       </c>
       <c r="F143" s="3">
-        <v>135</v>
+        <v>259</v>
       </c>
       <c r="G143" s="3">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="H143" s="1">
-        <v>2.3340000000000001</v>
+        <v>1.589</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -4383,206 +4652,24 @@
         <v>4.67</v>
       </c>
       <c r="B144" s="1">
-        <v>0.98399999999999999</v>
+        <v>4.258</v>
       </c>
       <c r="C144" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.108</v>
       </c>
       <c r="D144" s="2">
-        <v>331.95</v>
+        <v>331.75</v>
       </c>
       <c r="E144" s="2">
-        <v>334.15</v>
+        <v>339.34999999999997</v>
       </c>
       <c r="F144" s="3">
-        <v>171</v>
+        <v>275</v>
       </c>
       <c r="G144" s="3">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="H144" s="1">
-        <v>2.226</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B145" s="1">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="C145" s="1">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="D145" s="2">
-        <v>332.04999999999995</v>
-      </c>
-      <c r="E145" s="2">
-        <v>334.34999999999997</v>
-      </c>
-      <c r="F145" s="3">
-        <v>203</v>
-      </c>
-      <c r="G145" s="3">
-        <v>58</v>
-      </c>
-      <c r="H145" s="1">
-        <v>2.0459999999999998</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B146" s="1">
-        <v>1.6167</v>
-      </c>
-      <c r="C146" s="1">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="D146" s="2">
-        <v>331.65</v>
-      </c>
-      <c r="E146" s="2">
-        <v>334.34999999999997</v>
-      </c>
-      <c r="F146" s="3">
-        <v>204</v>
-      </c>
-      <c r="G146" s="3">
-        <v>64</v>
-      </c>
-      <c r="H146" s="1">
-        <v>1.9570000000000001</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B147" s="1">
-        <v>2.1019999999999999</v>
-      </c>
-      <c r="C147" s="1">
-        <v>5.5E-2</v>
-      </c>
-      <c r="D147" s="2">
-        <v>331.95</v>
-      </c>
-      <c r="E147" s="2">
-        <v>334.34999999999997</v>
-      </c>
-      <c r="F147" s="3">
-        <v>210</v>
-      </c>
-      <c r="G147" s="3">
-        <v>72</v>
-      </c>
-      <c r="H147" s="1">
-        <v>1.8220000000000001</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B148" s="1">
-        <v>2.621</v>
-      </c>
-      <c r="C148" s="1">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="D148" s="2">
-        <v>331.45</v>
-      </c>
-      <c r="E148" s="2">
-        <v>335.34999999999997</v>
-      </c>
-      <c r="F148" s="3">
-        <v>232</v>
-      </c>
-      <c r="G148" s="3">
-        <v>79</v>
-      </c>
-      <c r="H148" s="1">
-        <v>1.7070000000000001</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B149" s="1">
-        <v>3.1579999999999999</v>
-      </c>
-      <c r="C149" s="1">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D149" s="2">
-        <v>331.75</v>
-      </c>
-      <c r="E149" s="2">
-        <v>336.34999999999997</v>
-      </c>
-      <c r="F149" s="3">
-        <v>253</v>
-      </c>
-      <c r="G149" s="3">
-        <v>85</v>
-      </c>
-      <c r="H149" s="1">
-        <v>1.609</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B150" s="1">
-        <v>3.6949999999999998</v>
-      </c>
-      <c r="C150" s="1">
-        <v>9.4E-2</v>
-      </c>
-      <c r="D150" s="2">
-        <v>331.84999999999997</v>
-      </c>
-      <c r="E150" s="2">
-        <v>337.75</v>
-      </c>
-      <c r="F150" s="3">
-        <v>259</v>
-      </c>
-      <c r="G150" s="3">
-        <v>87</v>
-      </c>
-      <c r="H150" s="1">
-        <v>1.589</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
-        <v>4.67</v>
-      </c>
-      <c r="B151" s="1">
-        <v>4.258</v>
-      </c>
-      <c r="C151" s="1">
-        <v>0.108</v>
-      </c>
-      <c r="D151" s="2">
-        <v>331.75</v>
-      </c>
-      <c r="E151" s="2">
-        <v>339.34999999999997</v>
-      </c>
-      <c r="F151" s="3">
-        <v>275</v>
-      </c>
-      <c r="G151" s="3">
-        <v>91</v>
-      </c>
-      <c r="H151" s="1">
         <v>1.5069999999999999</v>
       </c>
     </row>

</xml_diff>